<commit_message>
cập nhật thời gian
</commit_message>
<xml_diff>
--- a/Đồ án CayNhiPhan.xlsx
+++ b/Đồ án CayNhiPhan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bich Ngoc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\cay-nhi-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19D1DFD-0DA1-43CB-A570-72F71F6ABEE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A69611C-33D9-41D5-B717-F487E14B75D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
   <si>
     <t>STT</t>
   </si>
@@ -272,6 +272,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -292,45 +331,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,8 +617,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -634,24 +634,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
@@ -674,363 +674,379 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="24" customFormat="1">
-      <c r="A3" s="9">
+    <row r="3" spans="1:10" s="17" customFormat="1">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-    </row>
-    <row r="4" spans="1:10" s="24" customFormat="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="21" t="s">
+      <c r="D3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" s="17" customFormat="1">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-    </row>
-    <row r="5" spans="1:10" s="24" customFormat="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="21" t="s">
+      <c r="D4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" s="17" customFormat="1">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="1:10" s="24" customFormat="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="21" t="s">
+      <c r="D5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" s="17" customFormat="1">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" s="20" customFormat="1">
-      <c r="A7" s="7">
+      <c r="D6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" s="13" customFormat="1">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="19" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="1:10" s="20" customFormat="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="17" t="s">
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" s="13" customFormat="1">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="19" t="s">
+      <c r="D8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" s="20" customFormat="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="17" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" s="13" customFormat="1">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="19" t="s">
+      <c r="D9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" spans="1:10" s="20" customFormat="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="17" t="s">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" s="13" customFormat="1">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="19" t="s">
+      <c r="D10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="1:10" s="20" customFormat="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="17" t="s">
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" s="13" customFormat="1">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="19" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="1:10" s="20" customFormat="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="17" t="s">
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" s="13" customFormat="1">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="19" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:10" s="20" customFormat="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="17" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" s="13" customFormat="1">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="19" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="1:10" s="16" customFormat="1">
-      <c r="A14" s="8">
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" s="9" customFormat="1">
+      <c r="A14" s="21">
         <v>3</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" s="16" customFormat="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="12" t="s">
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" s="9" customFormat="1">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="15" t="s">
+      <c r="D15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" s="16" customFormat="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="12" t="s">
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" s="9" customFormat="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="15" t="s">
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" s="16" customFormat="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="12" t="s">
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="D17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" s="16" customFormat="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="12" t="s">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" s="9" customFormat="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="15" t="s">
+      <c r="D18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" s="16" customFormat="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="12" t="s">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" s="9" customFormat="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="15" t="s">
+      <c r="D19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4">

</xml_diff>

<commit_message>
cập nhật lại thời gian
</commit_message>
<xml_diff>
--- a/Đồ án CayNhiPhan.xlsx
+++ b/Đồ án CayNhiPhan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\cay-nhi-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A69611C-33D9-41D5-B717-F487E14B75D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A0F60-C8C1-4F93-9D43-AAC4EA296F48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
   <si>
     <t>STT</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>30/9/2018</t>
+  </si>
+  <si>
+    <t>18/9/2018</t>
   </si>
 </sst>
 </file>
@@ -689,10 +692,10 @@
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -709,10 +712,10 @@
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -729,10 +732,10 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -749,10 +752,10 @@
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>

</xml_diff>

<commit_message>
Cập nhật lần cuối
</commit_message>
<xml_diff>
--- a/Đồ án CayNhiPhan.xlsx
+++ b/Đồ án CayNhiPhan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\cay-nhi-phan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\cay-nhi-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A0F60-C8C1-4F93-9D43-AAC4EA296F48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28F5C7A-A3D6-4CAB-ABAC-FAD5F4517F82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
   <si>
     <t>STT</t>
   </si>
@@ -124,13 +124,22 @@
     <t>20/9/2018</t>
   </si>
   <si>
-    <t>24/9/2018</t>
-  </si>
-  <si>
     <t>30/9/2018</t>
   </si>
   <si>
-    <t>18/9/2018</t>
+    <t>18/10/2018</t>
+  </si>
+  <si>
+    <t>21/10/2018</t>
+  </si>
+  <si>
+    <t>21/9/2018</t>
+  </si>
+  <si>
+    <t>28/9/2018</t>
+  </si>
+  <si>
+    <t>27/9/2018</t>
   </si>
 </sst>
 </file>
@@ -259,7 +268,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -334,6 +343,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,8 +644,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -692,10 +716,10 @@
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -712,10 +736,10 @@
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -732,10 +756,10 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -752,10 +776,10 @@
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -802,10 +826,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -824,10 +848,10 @@
         <v>9</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -846,10 +870,10 @@
         <v>9</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="G10" s="25">
+        <v>43200</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -865,11 +889,11 @@
       <c r="E11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>35</v>
+      <c r="F11" s="25">
+        <v>43230</v>
+      </c>
+      <c r="G11" s="25">
+        <v>43414</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -885,10 +909,10 @@
       <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="12" t="s">
+      <c r="F12" s="25">
+        <v>43444</v>
+      </c>
+      <c r="G12" s="26" t="s">
         <v>35</v>
       </c>
       <c r="H12" s="12"/>
@@ -905,10 +929,10 @@
       <c r="E13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="25">
+        <v>43444</v>
+      </c>
+      <c r="G13" s="26" t="s">
         <v>35</v>
       </c>
       <c r="H13" s="12"/>
@@ -932,10 +956,10 @@
         <v>9</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -954,10 +978,10 @@
         <v>9</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -976,10 +1000,10 @@
         <v>9</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="G16" s="27">
+        <v>43200</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -997,11 +1021,11 @@
       <c r="E17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>35</v>
+      <c r="F17" s="27">
+        <v>43230</v>
+      </c>
+      <c r="G17" s="27">
+        <v>43414</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1019,10 +1043,10 @@
       <c r="E18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="F18" s="27">
+        <v>43444</v>
+      </c>
+      <c r="G18" s="28" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="8"/>
@@ -1041,10 +1065,10 @@
       <c r="E19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="27">
+        <v>43444</v>
+      </c>
+      <c r="G19" s="28" t="s">
         <v>35</v>
       </c>
       <c r="H19" s="8"/>
@@ -1065,8 +1089,12 @@
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="29">
+        <v>43201</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>

</xml_diff>